<commit_message>
finish project 4 adding stlc and stlcc
</commit_message>
<xml_diff>
--- a/CITY- RAWDOCKET_ (STL County and City Pulls) (1).xlsx
+++ b/CITY- RAWDOCKET_ (STL County and City Pulls) (1).xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Felicia\Danniel- Programming Project\DOCKET PULL- STL &amp; CITY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\svr2012r2-1\users\Desktops\ctsstaff\Desktop\CapstoneProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492B0516-93E4-496E-B54C-4F6210C654FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294F7D63-A482-49A6-9A1B-57C5275D70EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2A51916B-DAB5-4F9E-84B6-999203422207}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2A51916B-DAB5-4F9E-84B6-999203422207}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet - 1" sheetId="1" r:id="rId1"/>
@@ -2522,29 +2522,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5671EE01-F0F8-4927-8DAC-1F99BE24D4CA}">
-  <dimension ref="A1:L161"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:R161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="J149" sqref="J149"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R1" activeCellId="3" sqref="O1:O1048576 P1:P1048576 Q1:Q1048576 R1:R1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.140625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2581,8 +2586,12 @@
       <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="5"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>605</v>
       </c>
@@ -2620,7 +2629,7 @@
         <v>2919.39</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>327</v>
       </c>
@@ -2658,7 +2667,7 @@
         <v>4068.71</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
@@ -2696,7 +2705,7 @@
         <v>1316.24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>380</v>
       </c>
@@ -2734,7 +2743,7 @@
         <v>3198.31</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>164</v>
       </c>
@@ -2772,7 +2781,7 @@
         <v>1665.52</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>584</v>
       </c>
@@ -2810,7 +2819,7 @@
         <v>625.42999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>628</v>
       </c>
@@ -2848,7 +2857,7 @@
         <v>499.5</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>628</v>
       </c>
@@ -2886,7 +2895,7 @@
         <v>1047.68</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>288</v>
       </c>
@@ -2924,7 +2933,7 @@
         <v>3528.28</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>297</v>
       </c>
@@ -2962,7 +2971,7 @@
         <v>1013.47</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>361</v>
       </c>
@@ -3000,7 +3009,7 @@
         <v>1192.5999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -3038,7 +3047,7 @@
         <v>2862.14</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>101</v>
       </c>
@@ -3076,7 +3085,7 @@
         <v>2334.86</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>133</v>
       </c>
@@ -3114,7 +3123,7 @@
         <v>1210.8399999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>341</v>
       </c>
@@ -3152,7 +3161,7 @@
         <v>2041.74</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>345</v>
       </c>
@@ -3190,7 +3199,7 @@
         <v>5865.83</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>396</v>
       </c>
@@ -3228,7 +3237,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>393</v>
       </c>
@@ -3266,7 +3275,7 @@
         <v>7422.65</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>624</v>
       </c>
@@ -3304,7 +3313,7 @@
         <v>2305.19</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>263</v>
       </c>
@@ -3342,7 +3351,7 @@
         <v>11556.49</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>642</v>
       </c>
@@ -3380,7 +3389,7 @@
         <v>580.13</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -3418,7 +3427,7 @@
         <v>2943.36</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
@@ -3456,7 +3465,7 @@
         <v>1840.93</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
@@ -3494,7 +3503,7 @@
         <v>1816.18</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>54</v>
       </c>
@@ -3532,7 +3541,7 @@
         <v>869.95</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>58</v>
       </c>
@@ -3570,7 +3579,7 @@
         <v>2512.4699999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>302</v>
       </c>
@@ -3608,7 +3617,7 @@
         <v>1977.16</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>476</v>
       </c>
@@ -3646,7 +3655,7 @@
         <v>1294.28</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>509</v>
       </c>
@@ -3684,7 +3693,7 @@
         <v>797.82</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>528</v>
       </c>
@@ -3722,7 +3731,7 @@
         <v>615.38</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>327</v>
       </c>
@@ -3760,7 +3769,7 @@
         <v>1106.43</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>559</v>
       </c>
@@ -3798,7 +3807,7 @@
         <v>691.6</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>563</v>
       </c>
@@ -3836,7 +3845,7 @@
         <v>772.37</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>566</v>
       </c>
@@ -3874,7 +3883,7 @@
         <v>583.79</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>589</v>
       </c>
@@ -3912,7 +3921,7 @@
         <v>1193.3399999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>646</v>
       </c>
@@ -3950,7 +3959,7 @@
         <v>39950.9</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>652</v>
       </c>
@@ -3988,7 +3997,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>670</v>
       </c>
@@ -4026,7 +4035,7 @@
         <v>1426.69</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>436</v>
       </c>
@@ -4064,7 +4073,7 @@
         <v>1825.75</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
@@ -4102,7 +4111,7 @@
         <v>3145.84</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>29</v>
       </c>
@@ -4140,7 +4149,7 @@
         <v>4451.3999999999996</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>62</v>
       </c>
@@ -4178,7 +4187,7 @@
         <v>-1.46</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>58</v>
       </c>
@@ -4216,7 +4225,7 @@
         <v>752.38</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>70</v>
       </c>
@@ -4254,7 +4263,7 @@
         <v>2831.15</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>74</v>
       </c>
@@ -4292,7 +4301,7 @@
         <v>744.07</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>97</v>
       </c>
@@ -4330,7 +4339,7 @@
         <v>135046.47</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>17</v>
       </c>
@@ -4368,7 +4377,7 @@
         <v>1419.84</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>127</v>
       </c>
@@ -4406,7 +4415,7 @@
         <v>12958.05</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>253</v>
       </c>
@@ -4444,7 +4453,7 @@
         <v>11853.98</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>315</v>
       </c>
@@ -4482,7 +4491,7 @@
         <v>1694.32</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>384</v>
       </c>
@@ -4520,7 +4529,7 @@
         <v>1024.07</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>404</v>
       </c>
@@ -4558,7 +4567,7 @@
         <v>1641.91</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>449</v>
       </c>
@@ -4596,7 +4605,7 @@
         <v>1015.2</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>457</v>
       </c>
@@ -4634,7 +4643,7 @@
         <v>1561.45</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>480</v>
       </c>
@@ -4672,7 +4681,7 @@
         <v>1697.71</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>484</v>
       </c>
@@ -4710,7 +4719,7 @@
         <v>920.69</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>488</v>
       </c>
@@ -4748,7 +4757,7 @@
         <v>6236.2</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>492</v>
       </c>
@@ -4786,7 +4795,7 @@
         <v>561.71</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>495</v>
       </c>
@@ -4824,7 +4833,7 @@
         <v>986.21</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>357</v>
       </c>
@@ -4862,7 +4871,7 @@
         <v>1126.8399999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>502</v>
       </c>
@@ -4900,7 +4909,7 @@
         <v>1100.4000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>506</v>
       </c>
@@ -4938,7 +4947,7 @@
         <v>953.48</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>513</v>
       </c>
@@ -4976,7 +4985,7 @@
         <v>799.71</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>517</v>
       </c>
@@ -5014,7 +5023,7 @@
         <v>1125.1600000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>521</v>
       </c>
@@ -5052,7 +5061,7 @@
         <v>828.16</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>524</v>
       </c>
@@ -5090,7 +5099,7 @@
         <v>1276.68</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>533</v>
       </c>
@@ -5128,7 +5137,7 @@
         <v>1639.39</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>537</v>
       </c>
@@ -5166,7 +5175,7 @@
         <v>1370.83</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>375</v>
       </c>
@@ -5204,7 +5213,7 @@
         <v>694.02</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>543</v>
       </c>
@@ -5242,7 +5251,7 @@
         <v>738.01</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>548</v>
       </c>
@@ -5280,7 +5289,7 @@
         <v>1306.8399999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>551</v>
       </c>
@@ -5318,7 +5327,7 @@
         <v>559.14</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>555</v>
       </c>
@@ -5356,7 +5365,7 @@
         <v>781.48</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>570</v>
       </c>
@@ -5394,7 +5403,7 @@
         <v>912.74</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>574</v>
       </c>
@@ -5432,7 +5441,7 @@
         <v>1411.26</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>577</v>
       </c>
@@ -5470,7 +5479,7 @@
         <v>1644.44</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>580</v>
       </c>
@@ -5508,7 +5517,7 @@
         <v>819.39</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>598</v>
       </c>
@@ -5546,7 +5555,7 @@
         <v>1027.5</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>616</v>
       </c>
@@ -5584,7 +5593,7 @@
         <v>6358.09</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>439</v>
       </c>
@@ -5622,7 +5631,7 @@
         <v>1136.6600000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>269</v>
       </c>
@@ -5660,7 +5669,7 @@
         <v>11045.87</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>689</v>
       </c>
@@ -5698,7 +5707,7 @@
         <v>14851.22</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>183</v>
       </c>
@@ -5736,7 +5745,7 @@
         <v>1251.26</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>205</v>
       </c>
@@ -5774,7 +5783,7 @@
         <v>2374.21</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>219</v>
       </c>
@@ -5812,7 +5821,7 @@
         <v>1400.35</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>353</v>
       </c>
@@ -5850,7 +5859,7 @@
         <v>3884.61</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>22</v>
       </c>
@@ -5888,7 +5897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>258</v>
       </c>
@@ -5926,7 +5935,7 @@
         <v>56605.3</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>694</v>
       </c>
@@ -5964,7 +5973,7 @@
         <v>737.2</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>698</v>
       </c>
@@ -6002,7 +6011,7 @@
         <v>512.46</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>701</v>
       </c>
@@ -6040,7 +6049,7 @@
         <v>11196.75</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>620</v>
       </c>
@@ -6078,7 +6087,7 @@
         <v>1541.07</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>105</v>
       </c>
@@ -6116,7 +6125,7 @@
         <v>709.77</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>419</v>
       </c>
@@ -6154,7 +6163,7 @@
         <v>1273.6400000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>684</v>
       </c>
@@ -6192,7 +6201,7 @@
         <v>1337.44</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>92</v>
       </c>
@@ -6230,7 +6239,7 @@
         <v>3835.41</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>138</v>
       </c>
@@ -6268,7 +6277,7 @@
         <v>3699.35</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>637</v>
       </c>
@@ -6306,7 +6315,7 @@
         <v>514.89</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>332</v>
       </c>
@@ -6344,7 +6353,7 @@
         <v>5018.78</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>467</v>
       </c>
@@ -6382,7 +6391,7 @@
         <v>1238.6500000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>58</v>
       </c>
@@ -6420,7 +6429,7 @@
         <v>664.5</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>78</v>
       </c>
@@ -6458,7 +6467,7 @@
         <v>4901.95</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>84</v>
       </c>
@@ -6496,7 +6505,7 @@
         <v>9775.0400000000009</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>88</v>
       </c>
@@ -6534,7 +6543,7 @@
         <v>14988.85</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>375</v>
       </c>
@@ -6572,7 +6581,7 @@
         <v>1048.3499999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>423</v>
       </c>
@@ -6610,7 +6619,7 @@
         <v>1711.72</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>431</v>
       </c>
@@ -6648,7 +6657,7 @@
         <v>1859.19</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>441</v>
       </c>
@@ -6686,7 +6695,7 @@
         <v>940.35</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>306</v>
       </c>
@@ -6724,7 +6733,7 @@
         <v>1816.83</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>157</v>
       </c>
@@ -6762,7 +6771,7 @@
         <v>4131.3500000000004</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>367</v>
       </c>
@@ -6800,7 +6809,7 @@
         <v>2339.9899999999998</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>371</v>
       </c>
@@ -6838,7 +6847,7 @@
         <v>4366.3599999999997</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>662</v>
       </c>
@@ -6876,7 +6885,7 @@
         <v>982.48</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>276</v>
       </c>
@@ -6914,7 +6923,7 @@
         <v>4753.8999999999996</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>111</v>
       </c>
@@ -6952,7 +6961,7 @@
         <v>3702.96</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>122</v>
       </c>
@@ -6990,7 +6999,7 @@
         <v>994.94</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
         <v>145</v>
       </c>
@@ -7028,7 +7037,7 @@
         <v>741.81</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>170</v>
       </c>
@@ -7066,7 +7075,7 @@
         <v>1972.35</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>175</v>
       </c>
@@ -7104,7 +7113,7 @@
         <v>1199.3399999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>179</v>
       </c>
@@ -7142,7 +7151,7 @@
         <v>1631.03</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="9" t="s">
         <v>190</v>
       </c>
@@ -7180,7 +7189,7 @@
         <v>975.16</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="9" t="s">
         <v>139</v>
       </c>
@@ -7218,7 +7227,7 @@
         <v>2604.46</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="9" t="s">
         <v>198</v>
       </c>
@@ -7256,7 +7265,7 @@
         <v>1135.21</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
         <v>12</v>
       </c>
@@ -7294,7 +7303,7 @@
         <v>1410.34</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="9" t="s">
         <v>210</v>
       </c>
@@ -7332,7 +7341,7 @@
         <v>1521.5</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="9" t="s">
         <v>215</v>
       </c>
@@ -7370,7 +7379,7 @@
         <v>2387.75</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="9" t="s">
         <v>282</v>
       </c>
@@ -7408,7 +7417,7 @@
         <v>3972.91</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
         <v>293</v>
       </c>
@@ -7446,7 +7455,7 @@
         <v>5000.71</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>306</v>
       </c>
@@ -7484,7 +7493,7 @@
         <v>2109.34</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>323</v>
       </c>
@@ -7522,7 +7531,7 @@
         <v>2544.89</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="9" t="s">
         <v>337</v>
       </c>
@@ -7560,7 +7569,7 @@
         <v>1945.61</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>349</v>
       </c>
@@ -7598,7 +7607,7 @@
         <v>4034.78</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="9" t="s">
         <v>357</v>
       </c>
@@ -7636,7 +7645,7 @@
         <v>1590.9</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="9" t="s">
         <v>388</v>
       </c>
@@ -7674,7 +7683,7 @@
         <v>1332.25</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>392</v>
       </c>
@@ -7712,7 +7721,7 @@
         <v>3472.24</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="9" t="s">
         <v>400</v>
       </c>
@@ -7750,7 +7759,7 @@
         <v>2474.9899999999998</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
         <v>17</v>
       </c>
@@ -7788,7 +7797,7 @@
         <v>4919.63</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="9" t="s">
         <v>445</v>
       </c>
@@ -7826,7 +7835,7 @@
         <v>3424.31</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="9" t="s">
         <v>611</v>
       </c>
@@ -7864,7 +7873,7 @@
         <v>966.78</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="9" t="s">
         <v>26</v>
       </c>
@@ -7902,7 +7911,7 @@
         <v>5647.99</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="9" t="s">
         <v>666</v>
       </c>
@@ -7940,7 +7949,7 @@
         <v>2265.9</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="9" t="s">
         <v>675</v>
       </c>
@@ -7978,7 +7987,7 @@
         <v>2369.85</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="9" t="s">
         <v>680</v>
       </c>
@@ -8016,7 +8025,7 @@
         <v>1344.28</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
         <v>149</v>
       </c>
@@ -8054,7 +8063,7 @@
         <v>2623.69</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
         <v>149</v>
       </c>
@@ -8092,7 +8101,7 @@
         <v>2152.09</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
         <v>223</v>
       </c>
@@ -8130,7 +8139,7 @@
         <v>2493.75</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
         <v>149</v>
       </c>
@@ -8168,7 +8177,7 @@
         <v>1754.88</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>230</v>
       </c>
@@ -8206,7 +8215,7 @@
         <v>3332.99</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>234</v>
       </c>
@@ -8244,7 +8253,7 @@
         <v>1874.28</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>238</v>
       </c>
@@ -8282,7 +8291,7 @@
         <v>1111.03</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>149</v>
       </c>
@@ -8320,7 +8329,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
         <v>245</v>
       </c>
@@ -8358,7 +8367,7 @@
         <v>11803.76</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
         <v>249</v>
       </c>
@@ -8396,7 +8405,7 @@
         <v>3682.57</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>310</v>
       </c>
@@ -8434,7 +8443,7 @@
         <v>1604.1</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>319</v>
       </c>
@@ -8472,7 +8481,7 @@
         <v>1201.8699999999999</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>408</v>
       </c>
@@ -8510,7 +8519,7 @@
         <v>3211.93</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>415</v>
       </c>
@@ -8548,7 +8557,7 @@
         <v>1838.26</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
         <v>419</v>
       </c>
@@ -8586,7 +8595,7 @@
         <v>1297.1300000000001</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>472</v>
       </c>
@@ -8624,7 +8633,7 @@
         <v>885.57</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>461</v>
       </c>

</xml_diff>